<commit_message>
AVn, Ond, Subject, Vr.. updates plus updated Documentation
</commit_message>
<xml_diff>
--- a/methods/TARSP Index Current.xlsx
+++ b/methods/TARSP Index Current.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Odijk101\Dropbox\jodijk\myprograms\python\sastacode\sastadev\methods\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\jodijk\myprograms\python\sastacode\sastadev\methods\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFF7D176-1168-420B-8E00-3F7EF69116BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07808E40-558F-43A9-85EA-E9EDBDD294F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1634,9 +1634,6 @@
     <t>//node[@pt="ww" and @rel="hd"  and parent::node[node[ @rel="vc" and (@cat="inf" or @cat="ppart")]]]</t>
   </si>
   <si>
-    <t>//node[@pt="vnw"  and @vwtype="aanw" and @lemma!="hier" and @lemma!="daar" and @lemma!="er" and @rel!="det" and (not(@positie) or @positie!="prenom") ]</t>
-  </si>
-  <si>
     <t>//node[node[@rel="cnj" and (@cat="smain" or @cat="sv1")] and node[@rel="crd" ]]</t>
   </si>
   <si>
@@ -1906,6 +1903,9 @@
   </si>
   <si>
     <t>//node[@lemma="hem" and @pt="vnw"]</t>
+  </si>
+  <si>
+    <t>//node[%AVn% ]</t>
   </si>
 </sst>
 </file>
@@ -2326,11 +2326,11 @@
   <dimension ref="A1:R155"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="117" zoomScaleNormal="117" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="G29" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="1" topLeftCell="G5" activePane="bottomRight" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
-      <selection pane="bottomRight" activeCell="K34" sqref="K34"/>
+      <selection pane="bottomRight" activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2417,7 +2417,7 @@
         <v>199</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>72</v>
@@ -2587,7 +2587,7 @@
         <v>1</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>520</v>
+        <v>591</v>
       </c>
       <c r="L6" s="2" t="s">
         <v>369</v>
@@ -2628,7 +2628,7 @@
         <v>1</v>
       </c>
       <c r="K7" s="3" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="L7" s="2" t="s">
         <v>370</v>
@@ -2742,7 +2742,7 @@
         <v>4</v>
       </c>
       <c r="K10" s="3" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="L10" s="3" t="s">
         <v>369</v>
@@ -2806,7 +2806,7 @@
         <v>40</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="H12" s="2" t="s">
         <v>369</v>
@@ -2818,7 +2818,7 @@
         <v>3</v>
       </c>
       <c r="K12" s="3" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="L12" s="2" t="s">
         <v>369</v>
@@ -2926,7 +2926,7 @@
         <v>4</v>
       </c>
       <c r="K15" s="3" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="L15" s="2" t="s">
         <v>369</v>
@@ -3066,7 +3066,7 @@
         <v>1</v>
       </c>
       <c r="K19" s="3" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="L19" s="2" t="s">
         <v>369</v>
@@ -3197,7 +3197,7 @@
         <v>49</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="H23" s="2" t="s">
         <v>369</v>
@@ -3209,7 +3209,7 @@
         <v>5</v>
       </c>
       <c r="K23" s="2" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="L23" s="2" t="s">
         <v>369</v>
@@ -3253,7 +3253,7 @@
         <v>2</v>
       </c>
       <c r="K24" s="3" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="L24" s="2" t="s">
         <v>369</v>
@@ -3265,7 +3265,7 @@
         <v>462</v>
       </c>
       <c r="Q24" s="3" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.3">
@@ -3323,7 +3323,7 @@
         <v>4</v>
       </c>
       <c r="K26" s="3" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="L26" s="3" t="s">
         <v>369</v>
@@ -3469,7 +3469,7 @@
         <v>3</v>
       </c>
       <c r="K30" s="2" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="L30" s="2" t="s">
         <v>369</v>
@@ -3621,7 +3621,7 @@
         <v>6</v>
       </c>
       <c r="K34" s="2" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="L34" s="2" t="s">
         <v>369</v>
@@ -3764,7 +3764,7 @@
         <v>380</v>
       </c>
       <c r="K38" s="3" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="L38" s="3" t="s">
         <v>369</v>
@@ -3802,7 +3802,7 @@
         <v>4</v>
       </c>
       <c r="K39" s="3" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="L39" s="3" t="s">
         <v>369</v>
@@ -3837,7 +3837,7 @@
         <v>3</v>
       </c>
       <c r="K40" s="3" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="L40" s="3" t="s">
         <v>369</v>
@@ -3957,7 +3957,7 @@
         <v>3</v>
       </c>
       <c r="K43" s="3" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="L43" s="2" t="s">
         <v>369</v>
@@ -3995,7 +3995,7 @@
         <v>3</v>
       </c>
       <c r="K44" s="2" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="L44" s="2" t="s">
         <v>369</v>
@@ -4071,7 +4071,7 @@
         <v>2</v>
       </c>
       <c r="K46" s="2" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="L46" s="2" t="s">
         <v>369</v>
@@ -4135,7 +4135,7 @@
         <v>370</v>
       </c>
       <c r="K48" s="3" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="L48" s="3" t="s">
         <v>370</v>
@@ -4354,7 +4354,7 @@
         <v>6</v>
       </c>
       <c r="K54" s="2" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="L54" s="2" t="s">
         <v>369</v>
@@ -4456,7 +4456,7 @@
         <v>1</v>
       </c>
       <c r="K57" s="3" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="L57" s="2" t="s">
         <v>370</v>
@@ -4497,7 +4497,7 @@
         <v>2</v>
       </c>
       <c r="K58" s="2" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="L58" s="2" t="s">
         <v>369</v>
@@ -4538,7 +4538,7 @@
         <v>3</v>
       </c>
       <c r="K59" s="2" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="L59" s="2" t="s">
         <v>369</v>
@@ -4766,7 +4766,7 @@
         <v>2</v>
       </c>
       <c r="K65" s="2" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="L65" s="2" t="s">
         <v>369</v>
@@ -4807,7 +4807,7 @@
         <v>2</v>
       </c>
       <c r="K66" s="2" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="L66" s="2" t="s">
         <v>369</v>
@@ -4848,7 +4848,7 @@
         <v>3</v>
       </c>
       <c r="K67" s="3" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="L67" s="2" t="s">
         <v>369</v>
@@ -4877,7 +4877,7 @@
         <v>46</v>
       </c>
       <c r="G68" s="2" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="H68" s="2" t="s">
         <v>369</v>
@@ -4971,7 +4971,7 @@
         <v>3</v>
       </c>
       <c r="K70" s="3" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="L70" s="2" t="s">
         <v>369</v>
@@ -5000,7 +5000,7 @@
         <v>48</v>
       </c>
       <c r="G71" s="2" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="H71" s="2" t="s">
         <v>369</v>
@@ -5012,7 +5012,7 @@
         <v>5</v>
       </c>
       <c r="K71" s="2" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="L71" s="2" t="s">
         <v>369</v>
@@ -5041,7 +5041,7 @@
         <v>425</v>
       </c>
       <c r="F72" s="2" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="H72" s="2" t="s">
         <v>369</v>
@@ -5079,7 +5079,7 @@
         <v>194</v>
       </c>
       <c r="F73" s="2" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="H73" s="2" t="s">
         <v>369</v>
@@ -5091,7 +5091,7 @@
         <v>3</v>
       </c>
       <c r="K73" s="2" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L73" s="2" t="s">
         <v>369</v>
@@ -5228,7 +5228,7 @@
         <v>51</v>
       </c>
       <c r="F77" s="2" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="H77" s="2" t="s">
         <v>369</v>
@@ -5240,7 +5240,7 @@
         <v>4</v>
       </c>
       <c r="K77" s="3" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="L77" s="2" t="s">
         <v>369</v>
@@ -5269,7 +5269,7 @@
         <v>50</v>
       </c>
       <c r="F78" s="2" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="H78" s="2" t="s">
         <v>369</v>
@@ -5281,7 +5281,7 @@
         <v>5</v>
       </c>
       <c r="K78" s="3" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="L78" s="2" t="s">
         <v>369</v>
@@ -5307,7 +5307,7 @@
         <v>141</v>
       </c>
       <c r="F79" s="2" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="H79" s="2" t="s">
         <v>369</v>
@@ -5392,7 +5392,7 @@
         <v>4</v>
       </c>
       <c r="K81" s="3" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="L81" s="3" t="s">
         <v>369</v>
@@ -5430,7 +5430,7 @@
         <v>4</v>
       </c>
       <c r="K82" s="3" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="L82" s="2" t="s">
         <v>369</v>
@@ -5616,7 +5616,7 @@
         <v>401</v>
       </c>
       <c r="F88" s="2" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="H88" s="2" t="s">
         <v>369</v>
@@ -5628,7 +5628,7 @@
         <v>1</v>
       </c>
       <c r="K88" s="3" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="L88" s="2" t="s">
         <v>369</v>
@@ -5724,7 +5724,7 @@
         <v>402</v>
       </c>
       <c r="F91" s="2" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="H91" s="2" t="s">
         <v>369</v>
@@ -5762,7 +5762,7 @@
         <v>369</v>
       </c>
       <c r="K92" s="2" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="L92" s="2" t="s">
         <v>370</v>
@@ -5803,7 +5803,7 @@
         <v>6</v>
       </c>
       <c r="K93" s="2" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="L93" s="2" t="s">
         <v>369</v>
@@ -5873,7 +5873,7 @@
         <v>47</v>
       </c>
       <c r="G95" s="2" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="H95" s="2" t="s">
         <v>369</v>
@@ -5885,7 +5885,7 @@
         <v>5</v>
       </c>
       <c r="K95" s="2" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="L95" s="2" t="s">
         <v>369</v>
@@ -5952,7 +5952,7 @@
         <v>471</v>
       </c>
       <c r="K97" s="3" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="L97" s="3" t="s">
         <v>369</v>
@@ -6098,7 +6098,7 @@
         <v>5</v>
       </c>
       <c r="K101" s="3" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="L101" s="2" t="s">
         <v>369</v>
@@ -6133,7 +6133,7 @@
         <v>4</v>
       </c>
       <c r="K102" s="2" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="L102" s="2" t="s">
         <v>369</v>
@@ -6282,7 +6282,7 @@
         <v>4</v>
       </c>
       <c r="K106" s="3" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="L106" s="2" t="s">
         <v>369</v>
@@ -6323,7 +6323,7 @@
         <v>5</v>
       </c>
       <c r="K107" s="3" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="L107" s="2" t="s">
         <v>369</v>
@@ -6364,7 +6364,7 @@
         <v>6</v>
       </c>
       <c r="K108" s="2" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="L108" s="2" t="s">
         <v>369</v>
@@ -6405,7 +6405,7 @@
         <v>6</v>
       </c>
       <c r="K109" s="3" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="L109" s="2" t="s">
         <v>369</v>
@@ -6509,7 +6509,7 @@
         <v>3</v>
       </c>
       <c r="K112" s="2" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="L112" s="2" t="s">
         <v>369</v>
@@ -6617,7 +6617,7 @@
         <v>1</v>
       </c>
       <c r="K115" s="3" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="L115" s="3" t="s">
         <v>369</v>
@@ -6781,7 +6781,7 @@
         <v>42</v>
       </c>
       <c r="G120" s="2" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="H120" s="2" t="s">
         <v>369</v>
@@ -6793,7 +6793,7 @@
         <v>3</v>
       </c>
       <c r="K120" s="3" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="L120" s="2" t="s">
         <v>369</v>
@@ -6939,7 +6939,7 @@
         <v>4</v>
       </c>
       <c r="K124" s="3" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="L124" s="2" t="s">
         <v>369</v>
@@ -6980,7 +6980,7 @@
         <v>5</v>
       </c>
       <c r="K125" s="2" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="L125" s="2" t="s">
         <v>369</v>
@@ -7024,7 +7024,7 @@
         <v>6</v>
       </c>
       <c r="K126" s="2" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="L126" s="2" t="s">
         <v>369</v>
@@ -7094,7 +7094,7 @@
         <v>6</v>
       </c>
       <c r="K128" s="2" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="L128" s="2" t="s">
         <v>369</v>
@@ -7167,7 +7167,7 @@
         <v>4</v>
       </c>
       <c r="K130" s="2" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="L130" s="2" t="s">
         <v>369</v>
@@ -7208,7 +7208,7 @@
         <v>5</v>
       </c>
       <c r="K131" s="2" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="L131" s="2" t="s">
         <v>369</v>
@@ -7252,7 +7252,7 @@
         <v>6</v>
       </c>
       <c r="K132" s="2" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="L132" s="2" t="s">
         <v>369</v>
@@ -7324,7 +7324,7 @@
       </c>
       <c r="F134" s="10"/>
       <c r="G134" s="10" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="H134" s="2" t="s">
         <v>369</v>
@@ -7404,7 +7404,7 @@
         <v>43</v>
       </c>
       <c r="G136" s="2" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="H136" s="2" t="s">
         <v>369</v>
@@ -7550,7 +7550,7 @@
         <v>1</v>
       </c>
       <c r="K140" s="3" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="L140" s="2" t="s">
         <v>369</v>
@@ -7611,7 +7611,7 @@
         <v>200</v>
       </c>
       <c r="E142" s="2" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="H142" s="2" t="s">
         <v>369</v>
@@ -7815,7 +7815,7 @@
         <v>429</v>
       </c>
       <c r="F148" s="2" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="H148" s="2" t="s">
         <v>369</v>

</xml_diff>

<commit_message>
updated basicreplacements and Vobij and Vo/bij
</commit_message>
<xml_diff>
--- a/methods/TARSP Index Current.xlsx
+++ b/methods/TARSP Index Current.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\jodijk\myprograms\python\sastacode\sastadev\methods\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07808E40-558F-43A9-85EA-E9EDBDD294F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10E75810-3B31-409B-8908-EB9B0F89935A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1672,13 +1672,6 @@
    ]</t>
   </si>
   <si>
-    <t>//node[node[@pt="vz" and @rel="hd"] and 
-            node[@rel="obj1" and 
-                 ((@index and not(@pt or @cat)) or
-                  (@end &lt; ../node[@rel="hd"]/@begin)
-                 )]]</t>
-  </si>
-  <si>
     <t>vu nee/ja, vu ja/nee,V.U. Ja/nee, nee, ja</t>
   </si>
   <si>
@@ -1862,9 +1855,6 @@
   </si>
   <si>
     <t>//node[%Tarsp_OndWB%]</t>
-  </si>
-  <si>
-    <t>//node[%Vobij%]</t>
   </si>
   <si>
     <t>//node[(@cat="top" and not(.//node[%pv%]) and not(.//node[@lemma="niet"]) and not(.//node[@rel="dlink"]) and
@@ -1906,6 +1896,12 @@
   </si>
   <si>
     <t>//node[%AVn% ]</t>
+  </si>
+  <si>
+    <t>vobij</t>
+  </si>
+  <si>
+    <t>voslashbij</t>
   </si>
 </sst>
 </file>
@@ -2326,11 +2322,11 @@
   <dimension ref="A1:R155"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="117" zoomScaleNormal="117" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="G5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="1" topLeftCell="G98" activePane="bottomRight" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
-      <selection pane="bottomRight" activeCell="K6" sqref="K6"/>
+      <selection pane="bottomRight" activeCell="K102" sqref="K102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2417,7 +2413,7 @@
         <v>199</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>72</v>
@@ -2587,7 +2583,7 @@
         <v>1</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="L6" s="2" t="s">
         <v>369</v>
@@ -2628,7 +2624,7 @@
         <v>1</v>
       </c>
       <c r="K7" s="3" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="L7" s="2" t="s">
         <v>370</v>
@@ -2806,7 +2802,7 @@
         <v>40</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="H12" s="2" t="s">
         <v>369</v>
@@ -2818,7 +2814,7 @@
         <v>3</v>
       </c>
       <c r="K12" s="3" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="L12" s="2" t="s">
         <v>369</v>
@@ -2926,7 +2922,7 @@
         <v>4</v>
       </c>
       <c r="K15" s="3" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="L15" s="2" t="s">
         <v>369</v>
@@ -3197,7 +3193,7 @@
         <v>49</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="H23" s="2" t="s">
         <v>369</v>
@@ -3209,7 +3205,7 @@
         <v>5</v>
       </c>
       <c r="K23" s="2" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="L23" s="2" t="s">
         <v>369</v>
@@ -3253,7 +3249,7 @@
         <v>2</v>
       </c>
       <c r="K24" s="3" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="L24" s="2" t="s">
         <v>369</v>
@@ -3265,7 +3261,7 @@
         <v>462</v>
       </c>
       <c r="Q24" s="3" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.3">
@@ -3323,7 +3319,7 @@
         <v>4</v>
       </c>
       <c r="K26" s="3" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="L26" s="3" t="s">
         <v>369</v>
@@ -3469,7 +3465,7 @@
         <v>3</v>
       </c>
       <c r="K30" s="2" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
       <c r="L30" s="2" t="s">
         <v>369</v>
@@ -3621,7 +3617,7 @@
         <v>6</v>
       </c>
       <c r="K34" s="2" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
       <c r="L34" s="2" t="s">
         <v>369</v>
@@ -3764,7 +3760,7 @@
         <v>380</v>
       </c>
       <c r="K38" s="3" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="L38" s="3" t="s">
         <v>369</v>
@@ -3802,7 +3798,7 @@
         <v>4</v>
       </c>
       <c r="K39" s="3" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="L39" s="3" t="s">
         <v>369</v>
@@ -3957,7 +3953,7 @@
         <v>3</v>
       </c>
       <c r="K43" s="3" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="L43" s="2" t="s">
         <v>369</v>
@@ -3995,7 +3991,7 @@
         <v>3</v>
       </c>
       <c r="K44" s="2" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="L44" s="2" t="s">
         <v>369</v>
@@ -4135,7 +4131,7 @@
         <v>370</v>
       </c>
       <c r="K48" s="3" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L48" s="3" t="s">
         <v>370</v>
@@ -4456,7 +4452,7 @@
         <v>1</v>
       </c>
       <c r="K57" s="3" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="L57" s="2" t="s">
         <v>370</v>
@@ -4497,7 +4493,7 @@
         <v>2</v>
       </c>
       <c r="K58" s="2" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="L58" s="2" t="s">
         <v>369</v>
@@ -4538,7 +4534,7 @@
         <v>3</v>
       </c>
       <c r="K59" s="2" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="L59" s="2" t="s">
         <v>369</v>
@@ -4766,7 +4762,7 @@
         <v>2</v>
       </c>
       <c r="K65" s="2" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="L65" s="2" t="s">
         <v>369</v>
@@ -4807,7 +4803,7 @@
         <v>2</v>
       </c>
       <c r="K66" s="2" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="L66" s="2" t="s">
         <v>369</v>
@@ -4848,7 +4844,7 @@
         <v>3</v>
       </c>
       <c r="K67" s="3" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="L67" s="2" t="s">
         <v>369</v>
@@ -4877,7 +4873,7 @@
         <v>46</v>
       </c>
       <c r="G68" s="2" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="H68" s="2" t="s">
         <v>369</v>
@@ -4971,7 +4967,7 @@
         <v>3</v>
       </c>
       <c r="K70" s="3" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="L70" s="2" t="s">
         <v>369</v>
@@ -5000,7 +4996,7 @@
         <v>48</v>
       </c>
       <c r="G71" s="2" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="H71" s="2" t="s">
         <v>369</v>
@@ -5012,7 +5008,7 @@
         <v>5</v>
       </c>
       <c r="K71" s="2" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="L71" s="2" t="s">
         <v>369</v>
@@ -5041,7 +5037,7 @@
         <v>425</v>
       </c>
       <c r="F72" s="2" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="H72" s="2" t="s">
         <v>369</v>
@@ -5079,7 +5075,7 @@
         <v>194</v>
       </c>
       <c r="F73" s="2" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="H73" s="2" t="s">
         <v>369</v>
@@ -5091,7 +5087,7 @@
         <v>3</v>
       </c>
       <c r="K73" s="2" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="L73" s="2" t="s">
         <v>369</v>
@@ -5228,7 +5224,7 @@
         <v>51</v>
       </c>
       <c r="F77" s="2" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="H77" s="2" t="s">
         <v>369</v>
@@ -5240,7 +5236,7 @@
         <v>4</v>
       </c>
       <c r="K77" s="3" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="L77" s="2" t="s">
         <v>369</v>
@@ -5269,7 +5265,7 @@
         <v>50</v>
       </c>
       <c r="F78" s="2" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="H78" s="2" t="s">
         <v>369</v>
@@ -5281,7 +5277,7 @@
         <v>5</v>
       </c>
       <c r="K78" s="3" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="L78" s="2" t="s">
         <v>369</v>
@@ -5307,7 +5303,7 @@
         <v>141</v>
       </c>
       <c r="F79" s="2" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="H79" s="2" t="s">
         <v>369</v>
@@ -5392,7 +5388,7 @@
         <v>4</v>
       </c>
       <c r="K81" s="3" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="L81" s="3" t="s">
         <v>369</v>
@@ -5616,7 +5612,7 @@
         <v>401</v>
       </c>
       <c r="F88" s="2" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="H88" s="2" t="s">
         <v>369</v>
@@ -5628,7 +5624,7 @@
         <v>1</v>
       </c>
       <c r="K88" s="3" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="L88" s="2" t="s">
         <v>369</v>
@@ -5724,7 +5720,7 @@
         <v>402</v>
       </c>
       <c r="F91" s="2" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="H91" s="2" t="s">
         <v>369</v>
@@ -5762,7 +5758,7 @@
         <v>369</v>
       </c>
       <c r="K92" s="2" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="L92" s="2" t="s">
         <v>370</v>
@@ -5803,7 +5799,7 @@
         <v>6</v>
       </c>
       <c r="K93" s="2" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="L93" s="2" t="s">
         <v>369</v>
@@ -5873,7 +5869,7 @@
         <v>47</v>
       </c>
       <c r="G95" s="2" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="H95" s="2" t="s">
         <v>369</v>
@@ -5885,7 +5881,7 @@
         <v>5</v>
       </c>
       <c r="K95" s="2" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="L95" s="2" t="s">
         <v>369</v>
@@ -5952,7 +5948,7 @@
         <v>471</v>
       </c>
       <c r="K97" s="3" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="L97" s="3" t="s">
         <v>369</v>
@@ -6075,7 +6071,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="101" spans="1:17" ht="72" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A101" s="2" t="s">
         <v>327</v>
       </c>
@@ -6098,7 +6094,7 @@
         <v>5</v>
       </c>
       <c r="K101" s="3" t="s">
-        <v>528</v>
+        <v>591</v>
       </c>
       <c r="L101" s="2" t="s">
         <v>369</v>
@@ -6133,7 +6129,7 @@
         <v>4</v>
       </c>
       <c r="K102" s="2" t="s">
-        <v>580</v>
+        <v>590</v>
       </c>
       <c r="L102" s="2" t="s">
         <v>369</v>
@@ -6282,7 +6278,7 @@
         <v>4</v>
       </c>
       <c r="K106" s="3" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="L106" s="2" t="s">
         <v>369</v>
@@ -6323,7 +6319,7 @@
         <v>5</v>
       </c>
       <c r="K107" s="3" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="L107" s="2" t="s">
         <v>369</v>
@@ -6364,7 +6360,7 @@
         <v>6</v>
       </c>
       <c r="K108" s="2" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="L108" s="2" t="s">
         <v>369</v>
@@ -6509,7 +6505,7 @@
         <v>3</v>
       </c>
       <c r="K112" s="2" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
       <c r="L112" s="2" t="s">
         <v>369</v>
@@ -6617,7 +6613,7 @@
         <v>1</v>
       </c>
       <c r="K115" s="3" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="L115" s="3" t="s">
         <v>369</v>
@@ -6781,7 +6777,7 @@
         <v>42</v>
       </c>
       <c r="G120" s="2" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="H120" s="2" t="s">
         <v>369</v>
@@ -6793,7 +6789,7 @@
         <v>3</v>
       </c>
       <c r="K120" s="3" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="L120" s="2" t="s">
         <v>369</v>
@@ -6939,7 +6935,7 @@
         <v>4</v>
       </c>
       <c r="K124" s="3" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="L124" s="2" t="s">
         <v>369</v>
@@ -6980,7 +6976,7 @@
         <v>5</v>
       </c>
       <c r="K125" s="2" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="L125" s="2" t="s">
         <v>369</v>
@@ -7024,7 +7020,7 @@
         <v>6</v>
       </c>
       <c r="K126" s="2" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="L126" s="2" t="s">
         <v>369</v>
@@ -7094,7 +7090,7 @@
         <v>6</v>
       </c>
       <c r="K128" s="2" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="L128" s="2" t="s">
         <v>369</v>
@@ -7167,7 +7163,7 @@
         <v>4</v>
       </c>
       <c r="K130" s="2" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="L130" s="2" t="s">
         <v>369</v>
@@ -7208,7 +7204,7 @@
         <v>5</v>
       </c>
       <c r="K131" s="2" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="L131" s="2" t="s">
         <v>369</v>
@@ -7252,7 +7248,7 @@
         <v>6</v>
       </c>
       <c r="K132" s="2" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="L132" s="2" t="s">
         <v>369</v>
@@ -7324,7 +7320,7 @@
       </c>
       <c r="F134" s="10"/>
       <c r="G134" s="10" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="H134" s="2" t="s">
         <v>369</v>
@@ -7404,7 +7400,7 @@
         <v>43</v>
       </c>
       <c r="G136" s="2" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="H136" s="2" t="s">
         <v>369</v>
@@ -7611,7 +7607,7 @@
         <v>200</v>
       </c>
       <c r="E142" s="2" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="H142" s="2" t="s">
         <v>369</v>
@@ -7815,7 +7811,7 @@
         <v>429</v>
       </c>
       <c r="F148" s="2" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="H148" s="2" t="s">
         <v>369</v>

</xml_diff>

<commit_message>
First version of Auchann Integration
</commit_message>
<xml_diff>
--- a/methods/TARSP Index Current.xlsx
+++ b/methods/TARSP Index Current.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\jodijk\myprograms\python\sastacode\sastadev\methods\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\jodijk\myprograms\python\sastacode\mysastadev\methods\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10E75810-3B31-409B-8908-EB9B0F89935A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD3DD31A-C98A-44BD-9F5D-9393ACD96900}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1163,9 +1163,6 @@
     <t>no</t>
   </si>
   <si>
-    <t>//node[@cat="pp" and node[ @rel="obj1" and node[@rel="det"] ]]</t>
-  </si>
-  <si>
     <t>//node[(@cat="ap" or @cat="advp" or @cat="np" or @cat="pp" or 
   node[@rel="vc" and (@cat="inf" or @cat="ppart")]) and parent::node[count(node[@cat or @pt!="let"])&gt;1]]</t>
   </si>
@@ -1902,6 +1899,9 @@
   </si>
   <si>
     <t>voslashbij</t>
+  </si>
+  <si>
+    <t>//node[@cat="pp" and node[@rel="hd"] and node[ @rel="obj1" and node[@rel="det"] ]]</t>
   </si>
 </sst>
 </file>
@@ -2326,7 +2326,7 @@
       <selection activeCell="C1" sqref="C1"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
-      <selection pane="bottomRight" activeCell="K102" sqref="K102"/>
+      <selection pane="bottomRight" activeCell="K111" sqref="K111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2381,19 +2381,19 @@
         <v>159</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="O1" s="1" t="s">
+        <v>472</v>
+      </c>
+      <c r="P1" s="1" t="s">
         <v>473</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>474</v>
       </c>
       <c r="Q1" s="1" t="s">
         <v>160</v>
@@ -2413,7 +2413,7 @@
         <v>199</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>72</v>
@@ -2437,10 +2437,10 @@
         <v>370</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.3">
@@ -2469,7 +2469,7 @@
         <v>6</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="L3" s="2" t="s">
         <v>369</v>
@@ -2478,10 +2478,10 @@
         <v>369</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="Q3" s="2" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.3">
@@ -2498,7 +2498,7 @@
         <v>199</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>65</v>
@@ -2519,7 +2519,7 @@
         <v>370</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.3">
@@ -2554,7 +2554,7 @@
         <v>370</v>
       </c>
       <c r="N5" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="Q5" s="2" t="s">
         <v>191</v>
@@ -2583,7 +2583,7 @@
         <v>1</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="L6" s="2" t="s">
         <v>369</v>
@@ -2592,13 +2592,13 @@
         <v>370</v>
       </c>
       <c r="N6" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="Q6" s="2" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="R6" s="2" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.3">
@@ -2624,7 +2624,7 @@
         <v>1</v>
       </c>
       <c r="K7" s="3" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="L7" s="2" t="s">
         <v>370</v>
@@ -2633,7 +2633,7 @@
         <v>370</v>
       </c>
       <c r="N7" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="8" spans="1:18" ht="115.2" x14ac:dyDescent="0.3">
@@ -2662,7 +2662,7 @@
         <v>4</v>
       </c>
       <c r="K8" s="3" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="L8" s="3" t="s">
         <v>370</v>
@@ -2671,7 +2671,7 @@
         <v>370</v>
       </c>
       <c r="N8" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.3">
@@ -2700,7 +2700,7 @@
         <v>6</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="L9" s="2" t="s">
         <v>369</v>
@@ -2709,10 +2709,10 @@
         <v>369</v>
       </c>
       <c r="N9" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="Q9" s="2" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="10" spans="1:18" ht="57.6" x14ac:dyDescent="0.3">
@@ -2738,7 +2738,7 @@
         <v>4</v>
       </c>
       <c r="K10" s="3" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="L10" s="3" t="s">
         <v>369</v>
@@ -2747,7 +2747,7 @@
         <v>370</v>
       </c>
       <c r="N10" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.3">
@@ -2782,7 +2782,7 @@
         <v>370</v>
       </c>
       <c r="N11" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.3">
@@ -2802,7 +2802,7 @@
         <v>40</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="H12" s="2" t="s">
         <v>369</v>
@@ -2814,7 +2814,7 @@
         <v>3</v>
       </c>
       <c r="K12" s="3" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="L12" s="2" t="s">
         <v>369</v>
@@ -2823,7 +2823,7 @@
         <v>370</v>
       </c>
       <c r="N12" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="13" spans="1:18" ht="57.6" x14ac:dyDescent="0.3">
@@ -2858,7 +2858,7 @@
         <v>370</v>
       </c>
       <c r="N13" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.3">
@@ -2887,7 +2887,7 @@
         <v>4</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="L14" s="2" t="s">
         <v>370</v>
@@ -2896,7 +2896,7 @@
         <v>370</v>
       </c>
       <c r="N14" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="15" spans="1:18" ht="86.4" x14ac:dyDescent="0.3">
@@ -2922,7 +2922,7 @@
         <v>4</v>
       </c>
       <c r="K15" s="3" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="L15" s="2" t="s">
         <v>369</v>
@@ -2931,7 +2931,7 @@
         <v>370</v>
       </c>
       <c r="N15" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.3">
@@ -2951,7 +2951,7 @@
         <v>369</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="L16" s="2" t="s">
         <v>370</v>
@@ -2960,7 +2960,7 @@
         <v>370</v>
       </c>
       <c r="N16" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.3">
@@ -2992,7 +2992,7 @@
         <v>369</v>
       </c>
       <c r="N17" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.3">
@@ -3009,10 +3009,10 @@
         <v>199</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="H18" s="2" t="s">
         <v>369</v>
@@ -3030,10 +3030,10 @@
         <v>370</v>
       </c>
       <c r="N18" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="O18" s="2" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="19" spans="1:17" ht="57.6" x14ac:dyDescent="0.3">
@@ -3047,7 +3047,7 @@
         <v>199</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="F19" s="2" t="s">
         <v>7</v>
@@ -3062,7 +3062,7 @@
         <v>1</v>
       </c>
       <c r="K19" s="3" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="L19" s="2" t="s">
         <v>369</v>
@@ -3071,7 +3071,7 @@
         <v>369</v>
       </c>
       <c r="N19" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.3">
@@ -3103,7 +3103,7 @@
         <v>370</v>
       </c>
       <c r="N20" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.3">
@@ -3129,7 +3129,7 @@
         <v>4</v>
       </c>
       <c r="K21" s="2" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="L21" s="2" t="s">
         <v>369</v>
@@ -3138,7 +3138,7 @@
         <v>370</v>
       </c>
       <c r="N21" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.3">
@@ -3164,7 +3164,7 @@
         <v>3</v>
       </c>
       <c r="K22" s="3" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="L22" s="2" t="s">
         <v>369</v>
@@ -3173,7 +3173,7 @@
         <v>370</v>
       </c>
       <c r="N22" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.3">
@@ -3193,7 +3193,7 @@
         <v>49</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="H23" s="2" t="s">
         <v>369</v>
@@ -3205,7 +3205,7 @@
         <v>5</v>
       </c>
       <c r="K23" s="2" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="L23" s="2" t="s">
         <v>369</v>
@@ -3214,7 +3214,7 @@
         <v>370</v>
       </c>
       <c r="N23" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="24" spans="1:17" ht="409.6" x14ac:dyDescent="0.3">
@@ -3231,7 +3231,7 @@
         <v>199</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="F24" s="2" t="s">
         <v>28</v>
@@ -3249,7 +3249,7 @@
         <v>2</v>
       </c>
       <c r="K24" s="3" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="L24" s="2" t="s">
         <v>369</v>
@@ -3258,10 +3258,10 @@
         <v>370</v>
       </c>
       <c r="N24" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="Q24" s="3" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.3">
@@ -3293,7 +3293,7 @@
         <v>370</v>
       </c>
       <c r="N25" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="26" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
@@ -3319,7 +3319,7 @@
         <v>4</v>
       </c>
       <c r="K26" s="3" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="L26" s="3" t="s">
         <v>369</v>
@@ -3328,10 +3328,10 @@
         <v>370</v>
       </c>
       <c r="N26" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="Q26" s="2" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.3">
@@ -3357,7 +3357,7 @@
         <v>4</v>
       </c>
       <c r="K27" s="2" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="L27" s="2" t="s">
         <v>369</v>
@@ -3366,7 +3366,7 @@
         <v>370</v>
       </c>
       <c r="N27" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.3">
@@ -3392,7 +3392,7 @@
         <v>5</v>
       </c>
       <c r="K28" s="2" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="L28" s="2" t="s">
         <v>369</v>
@@ -3401,7 +3401,7 @@
         <v>369</v>
       </c>
       <c r="N28" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.3">
@@ -3427,19 +3427,19 @@
         <v>2</v>
       </c>
       <c r="K29" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="L29" s="2" t="s">
+        <v>369</v>
+      </c>
+      <c r="M29" s="2" t="s">
+        <v>370</v>
+      </c>
+      <c r="N29" s="2" t="s">
+        <v>461</v>
+      </c>
+      <c r="Q29" s="2" t="s">
         <v>389</v>
-      </c>
-      <c r="L29" s="2" t="s">
-        <v>369</v>
-      </c>
-      <c r="M29" s="2" t="s">
-        <v>370</v>
-      </c>
-      <c r="N29" s="2" t="s">
-        <v>462</v>
-      </c>
-      <c r="Q29" s="2" t="s">
-        <v>390</v>
       </c>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.3">
@@ -3465,7 +3465,7 @@
         <v>3</v>
       </c>
       <c r="K30" s="2" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="L30" s="2" t="s">
         <v>369</v>
@@ -3474,7 +3474,7 @@
         <v>369</v>
       </c>
       <c r="N30" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="Q30" s="2" t="s">
         <v>191</v>
@@ -3512,7 +3512,7 @@
         <v>370</v>
       </c>
       <c r="N31" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="32" spans="1:17" ht="57.6" x14ac:dyDescent="0.3">
@@ -3529,7 +3529,7 @@
         <v>108</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="H32" s="2" t="s">
         <v>369</v>
@@ -3541,7 +3541,7 @@
         <v>6</v>
       </c>
       <c r="K32" s="3" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="L32" s="3" t="s">
         <v>369</v>
@@ -3550,7 +3550,7 @@
         <v>370</v>
       </c>
       <c r="N32" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.3">
@@ -3591,7 +3591,7 @@
         <v>370</v>
       </c>
       <c r="N33" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.3">
@@ -3617,7 +3617,7 @@
         <v>6</v>
       </c>
       <c r="K34" s="2" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="L34" s="2" t="s">
         <v>369</v>
@@ -3626,7 +3626,7 @@
         <v>370</v>
       </c>
       <c r="N34" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.3">
@@ -3661,7 +3661,7 @@
         <v>369</v>
       </c>
       <c r="N35" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="36" spans="1:17" ht="57.6" x14ac:dyDescent="0.3">
@@ -3687,7 +3687,7 @@
         <v>5</v>
       </c>
       <c r="K36" s="3" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="L36" s="3" t="s">
         <v>369</v>
@@ -3696,7 +3696,7 @@
         <v>369</v>
       </c>
       <c r="N36" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.3">
@@ -3722,7 +3722,7 @@
         <v>3</v>
       </c>
       <c r="K37" s="2" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="L37" s="2" t="s">
         <v>369</v>
@@ -3731,7 +3731,7 @@
         <v>370</v>
       </c>
       <c r="N37" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="38" spans="1:17" x14ac:dyDescent="0.3">
@@ -3757,10 +3757,10 @@
         <v>65</v>
       </c>
       <c r="J38" s="2" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="K38" s="3" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L38" s="3" t="s">
         <v>369</v>
@@ -3769,7 +3769,7 @@
         <v>370</v>
       </c>
       <c r="N38" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="39" spans="1:17" ht="100.8" x14ac:dyDescent="0.3">
@@ -3798,7 +3798,7 @@
         <v>4</v>
       </c>
       <c r="K39" s="3" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="L39" s="3" t="s">
         <v>369</v>
@@ -3807,7 +3807,7 @@
         <v>370</v>
       </c>
       <c r="N39" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.3">
@@ -3833,7 +3833,7 @@
         <v>3</v>
       </c>
       <c r="K40" s="3" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="L40" s="3" t="s">
         <v>369</v>
@@ -3842,10 +3842,10 @@
         <v>369</v>
       </c>
       <c r="N40" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="Q40" s="2" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
     </row>
     <row r="41" spans="1:17" x14ac:dyDescent="0.3">
@@ -3880,7 +3880,7 @@
         <v>369</v>
       </c>
       <c r="N41" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="42" spans="1:17" x14ac:dyDescent="0.3">
@@ -3900,7 +3900,7 @@
         <v>69</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="H42" s="2" t="s">
         <v>369</v>
@@ -3918,7 +3918,7 @@
         <v>370</v>
       </c>
       <c r="N42" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="Q42" s="2" t="s">
         <v>163</v>
@@ -3938,10 +3938,10 @@
         <v>199</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="H43" s="2" t="s">
         <v>369</v>
@@ -3953,7 +3953,7 @@
         <v>3</v>
       </c>
       <c r="K43" s="3" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="L43" s="2" t="s">
         <v>369</v>
@@ -3962,10 +3962,10 @@
         <v>370</v>
       </c>
       <c r="N43" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="Q43" s="2" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="44" spans="1:17" x14ac:dyDescent="0.3">
@@ -3991,7 +3991,7 @@
         <v>3</v>
       </c>
       <c r="K44" s="2" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="L44" s="2" t="s">
         <v>369</v>
@@ -4000,7 +4000,7 @@
         <v>370</v>
       </c>
       <c r="N44" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="45" spans="1:17" ht="57.6" x14ac:dyDescent="0.3">
@@ -4026,7 +4026,7 @@
         <v>6</v>
       </c>
       <c r="K45" s="3" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="L45" s="2" t="s">
         <v>369</v>
@@ -4035,7 +4035,7 @@
         <v>370</v>
       </c>
       <c r="N45" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="46" spans="1:17" x14ac:dyDescent="0.3">
@@ -4067,7 +4067,7 @@
         <v>2</v>
       </c>
       <c r="K46" s="2" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="L46" s="2" t="s">
         <v>369</v>
@@ -4076,7 +4076,7 @@
         <v>370</v>
       </c>
       <c r="N46" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="47" spans="1:17" ht="86.4" x14ac:dyDescent="0.3">
@@ -4102,7 +4102,7 @@
         <v>6</v>
       </c>
       <c r="K47" s="3" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="L47" s="2" t="s">
         <v>369</v>
@@ -4111,7 +4111,7 @@
         <v>370</v>
       </c>
       <c r="N47" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="Q47" s="2" t="s">
         <v>191</v>
@@ -4131,7 +4131,7 @@
         <v>370</v>
       </c>
       <c r="K48" s="3" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="L48" s="3" t="s">
         <v>370</v>
@@ -4140,7 +4140,7 @@
         <v>370</v>
       </c>
       <c r="N48" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="Q48" s="6" t="s">
         <v>186</v>
@@ -4178,7 +4178,7 @@
         <v>370</v>
       </c>
       <c r="N49" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="50" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
@@ -4204,7 +4204,7 @@
         <v>5</v>
       </c>
       <c r="K50" s="3" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="L50" s="2" t="s">
         <v>369</v>
@@ -4213,7 +4213,7 @@
         <v>370</v>
       </c>
       <c r="N50" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="51" spans="1:17" x14ac:dyDescent="0.3">
@@ -4248,7 +4248,7 @@
         <v>370</v>
       </c>
       <c r="N51" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="52" spans="1:17" x14ac:dyDescent="0.3">
@@ -4286,7 +4286,7 @@
         <v>370</v>
       </c>
       <c r="N52" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="53" spans="1:17" x14ac:dyDescent="0.3">
@@ -4312,7 +4312,7 @@
         <v>6</v>
       </c>
       <c r="K53" s="2" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="L53" s="2" t="s">
         <v>369</v>
@@ -4321,7 +4321,7 @@
         <v>370</v>
       </c>
       <c r="N53" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="54" spans="1:17" x14ac:dyDescent="0.3">
@@ -4350,7 +4350,7 @@
         <v>6</v>
       </c>
       <c r="K54" s="2" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="L54" s="2" t="s">
         <v>369</v>
@@ -4359,7 +4359,7 @@
         <v>370</v>
       </c>
       <c r="N54" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="55" spans="1:17" x14ac:dyDescent="0.3">
@@ -4394,7 +4394,7 @@
         <v>369</v>
       </c>
       <c r="N55" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="56" spans="1:17" x14ac:dyDescent="0.3">
@@ -4426,7 +4426,7 @@
         <v>370</v>
       </c>
       <c r="N56" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="57" spans="1:17" x14ac:dyDescent="0.3">
@@ -4452,7 +4452,7 @@
         <v>1</v>
       </c>
       <c r="K57" s="3" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="L57" s="2" t="s">
         <v>370</v>
@@ -4461,7 +4461,7 @@
         <v>370</v>
       </c>
       <c r="N57" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="58" spans="1:17" x14ac:dyDescent="0.3">
@@ -4493,7 +4493,7 @@
         <v>2</v>
       </c>
       <c r="K58" s="2" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="L58" s="2" t="s">
         <v>369</v>
@@ -4502,7 +4502,7 @@
         <v>369</v>
       </c>
       <c r="N58" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="59" spans="1:17" x14ac:dyDescent="0.3">
@@ -4534,7 +4534,7 @@
         <v>3</v>
       </c>
       <c r="K59" s="2" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="L59" s="2" t="s">
         <v>369</v>
@@ -4543,7 +4543,7 @@
         <v>370</v>
       </c>
       <c r="N59" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="60" spans="1:17" x14ac:dyDescent="0.3">
@@ -4560,7 +4560,7 @@
         <v>199</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="F60" s="2" t="s">
         <v>67</v>
@@ -4581,7 +4581,7 @@
         <v>370</v>
       </c>
       <c r="N60" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="61" spans="1:17" x14ac:dyDescent="0.3">
@@ -4616,10 +4616,10 @@
         <v>370</v>
       </c>
       <c r="N61" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="Q61" s="2" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="62" spans="1:17" x14ac:dyDescent="0.3">
@@ -4654,10 +4654,10 @@
         <v>370</v>
       </c>
       <c r="N62" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="Q62" s="2" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="63" spans="1:17" x14ac:dyDescent="0.3">
@@ -4692,10 +4692,10 @@
         <v>370</v>
       </c>
       <c r="N63" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="Q63" s="2" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="64" spans="1:17" x14ac:dyDescent="0.3">
@@ -4721,7 +4721,7 @@
         <v>4</v>
       </c>
       <c r="K64" s="2" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="L64" s="2" t="s">
         <v>370</v>
@@ -4730,7 +4730,7 @@
         <v>369</v>
       </c>
       <c r="N64" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="65" spans="1:17" x14ac:dyDescent="0.3">
@@ -4762,7 +4762,7 @@
         <v>2</v>
       </c>
       <c r="K65" s="2" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="L65" s="2" t="s">
         <v>369</v>
@@ -4771,7 +4771,7 @@
         <v>369</v>
       </c>
       <c r="N65" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="66" spans="1:17" x14ac:dyDescent="0.3">
@@ -4803,7 +4803,7 @@
         <v>2</v>
       </c>
       <c r="K66" s="2" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="L66" s="2" t="s">
         <v>369</v>
@@ -4812,7 +4812,7 @@
         <v>369</v>
       </c>
       <c r="N66" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="67" spans="1:17" x14ac:dyDescent="0.3">
@@ -4844,7 +4844,7 @@
         <v>3</v>
       </c>
       <c r="K67" s="3" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="L67" s="2" t="s">
         <v>369</v>
@@ -4853,7 +4853,7 @@
         <v>370</v>
       </c>
       <c r="N67" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="68" spans="1:17" x14ac:dyDescent="0.3">
@@ -4873,7 +4873,7 @@
         <v>46</v>
       </c>
       <c r="G68" s="2" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="H68" s="2" t="s">
         <v>369</v>
@@ -4885,7 +4885,7 @@
         <v>4</v>
       </c>
       <c r="K68" s="3" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="L68" s="2" t="s">
         <v>369</v>
@@ -4894,7 +4894,7 @@
         <v>370</v>
       </c>
       <c r="N68" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="69" spans="1:17" x14ac:dyDescent="0.3">
@@ -4926,7 +4926,7 @@
         <v>4</v>
       </c>
       <c r="K69" s="3" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="L69" s="2" t="s">
         <v>369</v>
@@ -4935,7 +4935,7 @@
         <v>369</v>
       </c>
       <c r="N69" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="70" spans="1:17" x14ac:dyDescent="0.3">
@@ -4967,7 +4967,7 @@
         <v>3</v>
       </c>
       <c r="K70" s="3" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="L70" s="2" t="s">
         <v>369</v>
@@ -4976,7 +4976,7 @@
         <v>369</v>
       </c>
       <c r="N70" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="71" spans="1:17" x14ac:dyDescent="0.3">
@@ -4996,7 +4996,7 @@
         <v>48</v>
       </c>
       <c r="G71" s="2" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="H71" s="2" t="s">
         <v>369</v>
@@ -5008,7 +5008,7 @@
         <v>5</v>
       </c>
       <c r="K71" s="2" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="L71" s="2" t="s">
         <v>369</v>
@@ -5017,7 +5017,7 @@
         <v>369</v>
       </c>
       <c r="N71" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="72" spans="1:17" x14ac:dyDescent="0.3">
@@ -5034,10 +5034,10 @@
         <v>199</v>
       </c>
       <c r="E72" s="2" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="F72" s="2" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="H72" s="2" t="s">
         <v>369</v>
@@ -5055,7 +5055,7 @@
         <v>370</v>
       </c>
       <c r="N72" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="73" spans="1:17" x14ac:dyDescent="0.3">
@@ -5075,7 +5075,7 @@
         <v>194</v>
       </c>
       <c r="F73" s="2" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="H73" s="2" t="s">
         <v>369</v>
@@ -5087,7 +5087,7 @@
         <v>3</v>
       </c>
       <c r="K73" s="2" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="L73" s="2" t="s">
         <v>369</v>
@@ -5096,7 +5096,7 @@
         <v>370</v>
       </c>
       <c r="N73" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="74" spans="1:17" x14ac:dyDescent="0.3">
@@ -5116,7 +5116,7 @@
         <v>195</v>
       </c>
       <c r="F74" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="H74" s="2" t="s">
         <v>369</v>
@@ -5134,7 +5134,7 @@
         <v>370</v>
       </c>
       <c r="N74" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="75" spans="1:17" x14ac:dyDescent="0.3">
@@ -5166,7 +5166,7 @@
         <v>370</v>
       </c>
       <c r="N75" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="76" spans="1:17" x14ac:dyDescent="0.3">
@@ -5183,7 +5183,7 @@
         <v>197</v>
       </c>
       <c r="F76" s="2" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="H76" s="2" t="s">
         <v>369</v>
@@ -5201,7 +5201,7 @@
         <v>370</v>
       </c>
       <c r="N76" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="Q76" s="2" t="s">
         <v>192</v>
@@ -5224,7 +5224,7 @@
         <v>51</v>
       </c>
       <c r="F77" s="2" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="H77" s="2" t="s">
         <v>369</v>
@@ -5236,7 +5236,7 @@
         <v>4</v>
       </c>
       <c r="K77" s="3" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="L77" s="2" t="s">
         <v>369</v>
@@ -5245,7 +5245,7 @@
         <v>370</v>
       </c>
       <c r="N77" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="78" spans="1:17" x14ac:dyDescent="0.3">
@@ -5265,7 +5265,7 @@
         <v>50</v>
       </c>
       <c r="F78" s="2" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="H78" s="2" t="s">
         <v>369</v>
@@ -5277,7 +5277,7 @@
         <v>5</v>
       </c>
       <c r="K78" s="3" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="L78" s="2" t="s">
         <v>369</v>
@@ -5286,7 +5286,7 @@
         <v>370</v>
       </c>
       <c r="N78" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="79" spans="1:17" x14ac:dyDescent="0.3">
@@ -5303,7 +5303,7 @@
         <v>141</v>
       </c>
       <c r="F79" s="2" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="H79" s="2" t="s">
         <v>369</v>
@@ -5315,7 +5315,7 @@
         <v>6</v>
       </c>
       <c r="K79" s="2" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="L79" s="2" t="s">
         <v>369</v>
@@ -5324,7 +5324,7 @@
         <v>370</v>
       </c>
       <c r="N79" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="80" spans="1:17" x14ac:dyDescent="0.3">
@@ -5359,7 +5359,7 @@
         <v>370</v>
       </c>
       <c r="N80" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="Q80" s="2" t="s">
         <v>168</v>
@@ -5388,7 +5388,7 @@
         <v>4</v>
       </c>
       <c r="K81" s="3" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="L81" s="3" t="s">
         <v>369</v>
@@ -5397,7 +5397,7 @@
         <v>370</v>
       </c>
       <c r="N81" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="82" spans="1:17" ht="86.4" x14ac:dyDescent="0.3">
@@ -5414,7 +5414,7 @@
         <v>152</v>
       </c>
       <c r="F82" s="2" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="H82" s="2" t="s">
         <v>369</v>
@@ -5426,7 +5426,7 @@
         <v>4</v>
       </c>
       <c r="K82" s="3" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="L82" s="2" t="s">
         <v>369</v>
@@ -5435,7 +5435,7 @@
         <v>370</v>
       </c>
       <c r="N82" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="83" spans="1:17" ht="115.2" x14ac:dyDescent="0.3">
@@ -5461,7 +5461,7 @@
         <v>370</v>
       </c>
       <c r="N83" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="84" spans="1:17" ht="115.2" x14ac:dyDescent="0.3">
@@ -5499,7 +5499,7 @@
         <v>370</v>
       </c>
       <c r="N84" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="85" spans="1:17" x14ac:dyDescent="0.3">
@@ -5531,7 +5531,7 @@
         <v>370</v>
       </c>
       <c r="N85" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="86" spans="1:17" x14ac:dyDescent="0.3">
@@ -5563,7 +5563,7 @@
         <v>370</v>
       </c>
       <c r="N86" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="87" spans="1:17" x14ac:dyDescent="0.3">
@@ -5595,7 +5595,7 @@
         <v>370</v>
       </c>
       <c r="N87" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="88" spans="1:17" ht="216" x14ac:dyDescent="0.3">
@@ -5609,10 +5609,10 @@
         <v>199</v>
       </c>
       <c r="E88" s="2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="F88" s="2" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="H88" s="2" t="s">
         <v>369</v>
@@ -5624,7 +5624,7 @@
         <v>1</v>
       </c>
       <c r="K88" s="3" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="L88" s="2" t="s">
         <v>369</v>
@@ -5633,7 +5633,7 @@
         <v>370</v>
       </c>
       <c r="N88" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="89" spans="1:17" x14ac:dyDescent="0.3">
@@ -5647,7 +5647,7 @@
         <v>199</v>
       </c>
       <c r="E89" s="2" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="H89" s="2" t="s">
         <v>369</v>
@@ -5659,7 +5659,7 @@
         <v>1</v>
       </c>
       <c r="K89" s="2" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="L89" s="2" t="s">
         <v>369</v>
@@ -5668,7 +5668,7 @@
         <v>370</v>
       </c>
       <c r="N89" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="90" spans="1:17" x14ac:dyDescent="0.3">
@@ -5682,10 +5682,10 @@
         <v>199</v>
       </c>
       <c r="E90" s="2" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="F90" s="2" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="H90" s="2" t="s">
         <v>369</v>
@@ -5703,12 +5703,12 @@
         <v>370</v>
       </c>
       <c r="N90" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="91" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A91" s="2" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="B91" s="2" t="s">
         <v>2</v>
@@ -5717,22 +5717,22 @@
         <v>199</v>
       </c>
       <c r="E91" s="2" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="F91" s="2" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="H91" s="2" t="s">
         <v>369</v>
       </c>
       <c r="I91" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="J91" s="2" t="s">
         <v>404</v>
       </c>
-      <c r="J91" s="2" t="s">
-        <v>405</v>
-      </c>
       <c r="K91" s="2" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="L91" s="2" t="s">
         <v>369</v>
@@ -5741,7 +5741,7 @@
         <v>370</v>
       </c>
       <c r="N91" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="92" spans="1:17" x14ac:dyDescent="0.3">
@@ -5758,7 +5758,7 @@
         <v>369</v>
       </c>
       <c r="K92" s="2" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="L92" s="2" t="s">
         <v>370</v>
@@ -5767,7 +5767,7 @@
         <v>370</v>
       </c>
       <c r="N92" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="93" spans="1:17" x14ac:dyDescent="0.3">
@@ -5787,7 +5787,7 @@
         <v>61</v>
       </c>
       <c r="F93" s="2" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="H93" s="2" t="s">
         <v>369</v>
@@ -5799,7 +5799,7 @@
         <v>6</v>
       </c>
       <c r="K93" s="2" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="L93" s="2" t="s">
         <v>369</v>
@@ -5808,7 +5808,7 @@
         <v>369</v>
       </c>
       <c r="N93" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="94" spans="1:17" x14ac:dyDescent="0.3">
@@ -5846,7 +5846,7 @@
         <v>369</v>
       </c>
       <c r="N94" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="Q94" s="2" t="s">
         <v>161</v>
@@ -5869,7 +5869,7 @@
         <v>47</v>
       </c>
       <c r="G95" s="2" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="H95" s="2" t="s">
         <v>369</v>
@@ -5881,7 +5881,7 @@
         <v>5</v>
       </c>
       <c r="K95" s="2" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="L95" s="2" t="s">
         <v>369</v>
@@ -5890,7 +5890,7 @@
         <v>369</v>
       </c>
       <c r="N95" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="96" spans="1:17" x14ac:dyDescent="0.3">
@@ -5916,7 +5916,7 @@
         <v>3</v>
       </c>
       <c r="K96" s="2" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="L96" s="2" t="s">
         <v>370</v>
@@ -5925,7 +5925,7 @@
         <v>369</v>
       </c>
       <c r="N96" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="97" spans="1:17" ht="129.6" x14ac:dyDescent="0.3">
@@ -5942,13 +5942,13 @@
         <v>369</v>
       </c>
       <c r="I97" s="2" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="J97" s="2" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="K97" s="3" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="L97" s="3" t="s">
         <v>369</v>
@@ -5957,7 +5957,7 @@
         <v>370</v>
       </c>
       <c r="N97" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="98" spans="1:17" x14ac:dyDescent="0.3">
@@ -5989,7 +5989,7 @@
         <v>370</v>
       </c>
       <c r="N98" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="99" spans="1:17" x14ac:dyDescent="0.3">
@@ -6003,7 +6003,7 @@
         <v>201</v>
       </c>
       <c r="E99" s="2" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="F99" s="2" t="s">
         <v>144</v>
@@ -6027,10 +6027,10 @@
         <v>370</v>
       </c>
       <c r="N99" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="O99" s="2" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="100" spans="1:17" x14ac:dyDescent="0.3">
@@ -6047,7 +6047,7 @@
         <v>155</v>
       </c>
       <c r="F100" s="2" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="H100" s="2" t="s">
         <v>369</v>
@@ -6059,7 +6059,7 @@
         <v>6</v>
       </c>
       <c r="K100" s="2" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="L100" s="2" t="s">
         <v>369</v>
@@ -6068,7 +6068,7 @@
         <v>369</v>
       </c>
       <c r="N100" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="101" spans="1:17" x14ac:dyDescent="0.3">
@@ -6094,7 +6094,7 @@
         <v>5</v>
       </c>
       <c r="K101" s="3" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="L101" s="2" t="s">
         <v>369</v>
@@ -6103,7 +6103,7 @@
         <v>370</v>
       </c>
       <c r="N101" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="102" spans="1:17" x14ac:dyDescent="0.3">
@@ -6129,7 +6129,7 @@
         <v>4</v>
       </c>
       <c r="K102" s="2" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="L102" s="2" t="s">
         <v>369</v>
@@ -6138,7 +6138,7 @@
         <v>370</v>
       </c>
       <c r="N102" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="103" spans="1:17" x14ac:dyDescent="0.3">
@@ -6176,7 +6176,7 @@
         <v>370</v>
       </c>
       <c r="N103" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="104" spans="1:17" x14ac:dyDescent="0.3">
@@ -6190,10 +6190,10 @@
         <v>201</v>
       </c>
       <c r="E104" s="2" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="F104" s="2" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="H104" s="2" t="s">
         <v>369</v>
@@ -6211,10 +6211,10 @@
         <v>370</v>
       </c>
       <c r="N104" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="O104" s="2" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="Q104" s="2" t="s">
         <v>172</v>
@@ -6234,19 +6234,19 @@
         <v>369</v>
       </c>
       <c r="K105" s="11" t="s">
+        <v>372</v>
+      </c>
+      <c r="L105" s="13" t="s">
+        <v>370</v>
+      </c>
+      <c r="M105" s="2" t="s">
+        <v>370</v>
+      </c>
+      <c r="N105" s="2" t="s">
+        <v>461</v>
+      </c>
+      <c r="Q105" s="2" t="s">
         <v>373</v>
-      </c>
-      <c r="L105" s="13" t="s">
-        <v>370</v>
-      </c>
-      <c r="M105" s="2" t="s">
-        <v>370</v>
-      </c>
-      <c r="N105" s="2" t="s">
-        <v>462</v>
-      </c>
-      <c r="Q105" s="2" t="s">
-        <v>374</v>
       </c>
     </row>
     <row r="106" spans="1:17" x14ac:dyDescent="0.3">
@@ -6266,7 +6266,7 @@
         <v>74</v>
       </c>
       <c r="F106" s="2" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="H106" s="2" t="s">
         <v>369</v>
@@ -6278,7 +6278,7 @@
         <v>4</v>
       </c>
       <c r="K106" s="3" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="L106" s="2" t="s">
         <v>369</v>
@@ -6287,7 +6287,7 @@
         <v>370</v>
       </c>
       <c r="N106" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="Q106" s="2" t="s">
         <v>165</v>
@@ -6319,7 +6319,7 @@
         <v>5</v>
       </c>
       <c r="K107" s="3" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="L107" s="2" t="s">
         <v>369</v>
@@ -6328,10 +6328,10 @@
         <v>370</v>
       </c>
       <c r="N107" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="Q107" s="2" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="108" spans="1:17" x14ac:dyDescent="0.3">
@@ -6360,7 +6360,7 @@
         <v>6</v>
       </c>
       <c r="K108" s="2" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="L108" s="2" t="s">
         <v>369</v>
@@ -6369,10 +6369,10 @@
         <v>369</v>
       </c>
       <c r="N108" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="O108" s="2" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="Q108" s="2" t="s">
         <v>165</v>
@@ -6401,7 +6401,7 @@
         <v>6</v>
       </c>
       <c r="K109" s="3" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="L109" s="2" t="s">
         <v>369</v>
@@ -6410,7 +6410,7 @@
         <v>370</v>
       </c>
       <c r="N109" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="110" spans="1:17" x14ac:dyDescent="0.3">
@@ -6443,7 +6443,7 @@
         <v>370</v>
       </c>
       <c r="N110" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="111" spans="1:17" x14ac:dyDescent="0.3">
@@ -6469,7 +6469,7 @@
         <v>4</v>
       </c>
       <c r="K111" s="2" t="s">
-        <v>371</v>
+        <v>591</v>
       </c>
       <c r="L111" s="2" t="s">
         <v>369</v>
@@ -6478,7 +6478,7 @@
         <v>369</v>
       </c>
       <c r="N111" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="112" spans="1:17" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -6505,7 +6505,7 @@
         <v>3</v>
       </c>
       <c r="K112" s="2" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="L112" s="2" t="s">
         <v>369</v>
@@ -6514,10 +6514,10 @@
         <v>370</v>
       </c>
       <c r="N112" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="Q112" s="3" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
     </row>
     <row r="113" spans="1:17" x14ac:dyDescent="0.3">
@@ -6552,7 +6552,7 @@
         <v>370</v>
       </c>
       <c r="N113" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="114" spans="1:17" x14ac:dyDescent="0.3">
@@ -6566,7 +6566,7 @@
         <v>199</v>
       </c>
       <c r="E114" s="2" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="H114" s="2" t="s">
         <v>369</v>
@@ -6587,7 +6587,7 @@
         <v>369</v>
       </c>
       <c r="N114" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="115" spans="1:17" x14ac:dyDescent="0.3">
@@ -6613,7 +6613,7 @@
         <v>1</v>
       </c>
       <c r="K115" s="3" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="L115" s="3" t="s">
         <v>369</v>
@@ -6622,10 +6622,10 @@
         <v>370</v>
       </c>
       <c r="N115" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="Q115" s="2" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="116" spans="1:17" x14ac:dyDescent="0.3">
@@ -6657,7 +6657,7 @@
         <v>3</v>
       </c>
       <c r="K116" s="2" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="L116" s="2" t="s">
         <v>369</v>
@@ -6666,7 +6666,7 @@
         <v>370</v>
       </c>
       <c r="N116" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="117" spans="1:17" x14ac:dyDescent="0.3">
@@ -6677,7 +6677,7 @@
         <v>199</v>
       </c>
       <c r="E117" s="4" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="F117" s="4"/>
       <c r="G117" s="4"/>
@@ -6694,7 +6694,7 @@
         <v>370</v>
       </c>
       <c r="N117" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="118" spans="1:17" x14ac:dyDescent="0.3">
@@ -6719,7 +6719,7 @@
         <v>370</v>
       </c>
       <c r="N118" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="119" spans="1:17" x14ac:dyDescent="0.3">
@@ -6754,7 +6754,7 @@
         <v>370</v>
       </c>
       <c r="N119" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="Q119" s="2" t="s">
         <v>191</v>
@@ -6777,7 +6777,7 @@
         <v>42</v>
       </c>
       <c r="G120" s="2" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="H120" s="2" t="s">
         <v>369</v>
@@ -6789,7 +6789,7 @@
         <v>3</v>
       </c>
       <c r="K120" s="3" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="L120" s="2" t="s">
         <v>369</v>
@@ -6798,7 +6798,7 @@
         <v>370</v>
       </c>
       <c r="N120" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="121" spans="1:17" x14ac:dyDescent="0.3">
@@ -6824,7 +6824,7 @@
         <v>4</v>
       </c>
       <c r="K121" s="2" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="L121" s="2" t="s">
         <v>369</v>
@@ -6833,7 +6833,7 @@
         <v>370</v>
       </c>
       <c r="N121" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="122" spans="1:17" x14ac:dyDescent="0.3">
@@ -6859,7 +6859,7 @@
         <v>3</v>
       </c>
       <c r="K122" s="2" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="L122" s="2" t="s">
         <v>370</v>
@@ -6868,7 +6868,7 @@
         <v>369</v>
       </c>
       <c r="N122" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="123" spans="1:17" x14ac:dyDescent="0.3">
@@ -6903,7 +6903,7 @@
         <v>369</v>
       </c>
       <c r="N123" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="124" spans="1:17" x14ac:dyDescent="0.3">
@@ -6935,7 +6935,7 @@
         <v>4</v>
       </c>
       <c r="K124" s="3" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="L124" s="2" t="s">
         <v>369</v>
@@ -6944,7 +6944,7 @@
         <v>370</v>
       </c>
       <c r="N124" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="125" spans="1:17" x14ac:dyDescent="0.3">
@@ -6976,7 +6976,7 @@
         <v>5</v>
       </c>
       <c r="K125" s="2" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="L125" s="2" t="s">
         <v>369</v>
@@ -6985,10 +6985,10 @@
         <v>370</v>
       </c>
       <c r="N125" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="Q125" s="2" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="126" spans="1:17" x14ac:dyDescent="0.3">
@@ -7020,7 +7020,7 @@
         <v>6</v>
       </c>
       <c r="K126" s="2" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="L126" s="2" t="s">
         <v>369</v>
@@ -7029,7 +7029,7 @@
         <v>369</v>
       </c>
       <c r="N126" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="127" spans="1:17" ht="86.4" x14ac:dyDescent="0.3">
@@ -7052,7 +7052,7 @@
         <v>188</v>
       </c>
       <c r="K127" s="3" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="L127" s="3" t="s">
         <v>370</v>
@@ -7061,7 +7061,7 @@
         <v>370</v>
       </c>
       <c r="N127" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="Q127" s="2" t="s">
         <v>190</v>
@@ -7090,7 +7090,7 @@
         <v>6</v>
       </c>
       <c r="K128" s="2" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="L128" s="2" t="s">
         <v>369</v>
@@ -7099,7 +7099,7 @@
         <v>370</v>
       </c>
       <c r="N128" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="129" spans="1:17" x14ac:dyDescent="0.3">
@@ -7131,7 +7131,7 @@
         <v>370</v>
       </c>
       <c r="N129" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="130" spans="1:17" x14ac:dyDescent="0.3">
@@ -7163,7 +7163,7 @@
         <v>4</v>
       </c>
       <c r="K130" s="2" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="L130" s="2" t="s">
         <v>369</v>
@@ -7172,7 +7172,7 @@
         <v>370</v>
       </c>
       <c r="N130" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="131" spans="1:17" x14ac:dyDescent="0.3">
@@ -7204,7 +7204,7 @@
         <v>5</v>
       </c>
       <c r="K131" s="2" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="L131" s="2" t="s">
         <v>369</v>
@@ -7213,7 +7213,7 @@
         <v>370</v>
       </c>
       <c r="N131" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="132" spans="1:17" x14ac:dyDescent="0.3">
@@ -7233,7 +7233,7 @@
         <v>84</v>
       </c>
       <c r="F132" s="2" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="G132" s="2" t="s">
         <v>8</v>
@@ -7248,7 +7248,7 @@
         <v>6</v>
       </c>
       <c r="K132" s="2" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="L132" s="2" t="s">
         <v>369</v>
@@ -7257,10 +7257,10 @@
         <v>370</v>
       </c>
       <c r="N132" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="O132" s="2" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="133" spans="1:17" x14ac:dyDescent="0.3">
@@ -7277,7 +7277,7 @@
         <v>107</v>
       </c>
       <c r="F133" s="10" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="G133" s="10"/>
       <c r="H133" s="2" t="s">
@@ -7290,7 +7290,7 @@
         <v>6</v>
       </c>
       <c r="K133" s="3" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="L133" s="2" t="s">
         <v>369</v>
@@ -7299,7 +7299,7 @@
         <v>370</v>
       </c>
       <c r="N133" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="134" spans="1:17" x14ac:dyDescent="0.3">
@@ -7320,7 +7320,7 @@
       </c>
       <c r="F134" s="10"/>
       <c r="G134" s="10" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="H134" s="2" t="s">
         <v>369</v>
@@ -7338,7 +7338,7 @@
         <v>370</v>
       </c>
       <c r="N134" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="135" spans="1:17" ht="115.2" x14ac:dyDescent="0.3">
@@ -7371,7 +7371,7 @@
         <v>3</v>
       </c>
       <c r="K135" s="3" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="L135" s="2" t="s">
         <v>369</v>
@@ -7380,7 +7380,7 @@
         <v>370</v>
       </c>
       <c r="N135" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="136" spans="1:17" x14ac:dyDescent="0.3">
@@ -7400,7 +7400,7 @@
         <v>43</v>
       </c>
       <c r="G136" s="2" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="H136" s="2" t="s">
         <v>369</v>
@@ -7418,7 +7418,7 @@
         <v>370</v>
       </c>
       <c r="N136" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="137" spans="1:17" x14ac:dyDescent="0.3">
@@ -7444,7 +7444,7 @@
         <v>4</v>
       </c>
       <c r="K137" s="2" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="L137" s="2" t="s">
         <v>369</v>
@@ -7453,7 +7453,7 @@
         <v>370</v>
       </c>
       <c r="N137" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="138" spans="1:17" x14ac:dyDescent="0.3">
@@ -7482,10 +7482,10 @@
         <v>370</v>
       </c>
       <c r="N138" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="Q138" s="2" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="139" spans="1:17" ht="72" x14ac:dyDescent="0.3">
@@ -7511,7 +7511,7 @@
         <v>7</v>
       </c>
       <c r="K139" s="3" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="L139" s="2" t="s">
         <v>369</v>
@@ -7520,7 +7520,7 @@
         <v>370</v>
       </c>
       <c r="N139" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="140" spans="1:17" ht="115.2" x14ac:dyDescent="0.3">
@@ -7546,7 +7546,7 @@
         <v>1</v>
       </c>
       <c r="K140" s="3" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="L140" s="2" t="s">
         <v>369</v>
@@ -7555,7 +7555,7 @@
         <v>369</v>
       </c>
       <c r="N140" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="141" spans="1:17" ht="86.4" x14ac:dyDescent="0.3">
@@ -7590,7 +7590,7 @@
         <v>370</v>
       </c>
       <c r="N141" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="Q141" s="2" t="s">
         <v>203</v>
@@ -7598,7 +7598,7 @@
     </row>
     <row r="142" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A142" s="2" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="B142" s="2" t="s">
         <v>85</v>
@@ -7607,51 +7607,51 @@
         <v>200</v>
       </c>
       <c r="E142" s="2" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="H142" s="2" t="s">
         <v>369</v>
       </c>
       <c r="I142" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="J142" s="2" t="s">
+        <v>404</v>
+      </c>
+      <c r="L142" s="2" t="s">
+        <v>370</v>
+      </c>
+      <c r="M142" s="2" t="s">
+        <v>370</v>
+      </c>
+      <c r="N142" s="2" t="s">
+        <v>461</v>
+      </c>
+      <c r="Q142" s="12" t="s">
         <v>378</v>
-      </c>
-      <c r="J142" s="2" t="s">
-        <v>405</v>
-      </c>
-      <c r="L142" s="2" t="s">
-        <v>370</v>
-      </c>
-      <c r="M142" s="2" t="s">
-        <v>370</v>
-      </c>
-      <c r="N142" s="2" t="s">
-        <v>462</v>
-      </c>
-      <c r="Q142" s="12" t="s">
-        <v>379</v>
       </c>
     </row>
     <row r="143" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A143" s="2" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B143" s="2" t="s">
+        <v>415</v>
+      </c>
+      <c r="E143" s="2" t="s">
         <v>416</v>
       </c>
-      <c r="E143" s="2" t="s">
+      <c r="H143" s="2" t="s">
+        <v>369</v>
+      </c>
+      <c r="I143" s="2" t="s">
         <v>417</v>
       </c>
-      <c r="H143" s="2" t="s">
-        <v>369</v>
-      </c>
-      <c r="I143" s="2" t="s">
-        <v>418</v>
-      </c>
       <c r="J143" s="2" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="K143" s="2" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="L143" s="2" t="s">
         <v>369</v>
@@ -7660,97 +7660,97 @@
         <v>370</v>
       </c>
       <c r="N143" s="2" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="Q143" s="2" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="144" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A144" s="2" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B144" s="2" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="E144" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="H144" s="2" t="s">
+        <v>369</v>
+      </c>
+      <c r="I144" s="2" t="s">
         <v>413</v>
       </c>
-      <c r="H144" s="2" t="s">
-        <v>369</v>
-      </c>
-      <c r="I144" s="2" t="s">
+      <c r="K144" s="2" t="s">
+        <v>468</v>
+      </c>
+      <c r="L144" s="2" t="s">
+        <v>369</v>
+      </c>
+      <c r="M144" s="2" t="s">
+        <v>370</v>
+      </c>
+      <c r="N144" s="2" t="s">
+        <v>462</v>
+      </c>
+      <c r="Q144" s="2" t="s">
         <v>414</v>
-      </c>
-      <c r="K144" s="2" t="s">
-        <v>469</v>
-      </c>
-      <c r="L144" s="2" t="s">
-        <v>369</v>
-      </c>
-      <c r="M144" s="2" t="s">
-        <v>370</v>
-      </c>
-      <c r="N144" s="2" t="s">
-        <v>463</v>
-      </c>
-      <c r="Q144" s="2" t="s">
-        <v>415</v>
       </c>
     </row>
     <row r="145" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A145" s="2" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B145" s="2" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="E145" s="2" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="H145" s="2" t="s">
         <v>369</v>
       </c>
       <c r="I145" s="2" t="s">
+        <v>413</v>
+      </c>
+      <c r="K145" s="2" t="s">
+        <v>467</v>
+      </c>
+      <c r="L145" s="2" t="s">
+        <v>369</v>
+      </c>
+      <c r="M145" s="2" t="s">
+        <v>370</v>
+      </c>
+      <c r="N145" s="2" t="s">
+        <v>462</v>
+      </c>
+      <c r="Q145" s="2" t="s">
         <v>414</v>
-      </c>
-      <c r="K145" s="2" t="s">
-        <v>468</v>
-      </c>
-      <c r="L145" s="2" t="s">
-        <v>369</v>
-      </c>
-      <c r="M145" s="2" t="s">
-        <v>370</v>
-      </c>
-      <c r="N145" s="2" t="s">
-        <v>463</v>
-      </c>
-      <c r="Q145" s="2" t="s">
-        <v>415</v>
       </c>
     </row>
     <row r="146" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A146" s="2" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="B146" s="2" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="E146" s="2" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="H146" s="2" t="s">
         <v>369</v>
       </c>
       <c r="I146" s="2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="J146" s="2" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="K146" s="2" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="L146" s="2" t="s">
         <v>369</v>
@@ -7759,33 +7759,33 @@
         <v>370</v>
       </c>
       <c r="N146" s="2" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="Q146" s="2" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="147" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A147" s="2" t="s">
+        <v>477</v>
+      </c>
+      <c r="B147" s="2" t="s">
+        <v>415</v>
+      </c>
+      <c r="E147" s="2" t="s">
         <v>478</v>
       </c>
-      <c r="B147" s="2" t="s">
-        <v>416</v>
-      </c>
-      <c r="E147" s="2" t="s">
-        <v>479</v>
-      </c>
       <c r="H147" s="2" t="s">
         <v>369</v>
       </c>
       <c r="I147" s="2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="J147" s="2" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="K147" s="2" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="L147" s="2" t="s">
         <v>369</v>
@@ -7794,34 +7794,34 @@
         <v>370</v>
       </c>
       <c r="N147" s="2" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="148" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A148" s="2" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="B148" s="2" t="s">
         <v>85</v>
       </c>
       <c r="D148" s="2" t="s">
+        <v>427</v>
+      </c>
+      <c r="E148" s="2" t="s">
         <v>428</v>
       </c>
-      <c r="E148" s="2" t="s">
+      <c r="F148" s="2" t="s">
+        <v>581</v>
+      </c>
+      <c r="H148" s="2" t="s">
+        <v>369</v>
+      </c>
+      <c r="I148" s="2" t="s">
         <v>429</v>
       </c>
-      <c r="F148" s="2" t="s">
-        <v>582</v>
-      </c>
-      <c r="H148" s="2" t="s">
-        <v>369</v>
-      </c>
-      <c r="I148" s="2" t="s">
+      <c r="J148" s="2" t="s">
         <v>430</v>
       </c>
-      <c r="J148" s="2" t="s">
-        <v>431</v>
-      </c>
       <c r="L148" s="2" t="s">
         <v>369</v>
       </c>
@@ -7829,28 +7829,28 @@
         <v>370</v>
       </c>
       <c r="N148" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="149" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A149" s="2" t="s">
+        <v>463</v>
+      </c>
+      <c r="B149" s="2" t="s">
+        <v>415</v>
+      </c>
+      <c r="E149" s="2" t="s">
+        <v>395</v>
+      </c>
+      <c r="H149" s="2" t="s">
+        <v>370</v>
+      </c>
+      <c r="I149" s="2" t="s">
         <v>464</v>
       </c>
-      <c r="B149" s="2" t="s">
-        <v>416</v>
-      </c>
-      <c r="E149" s="2" t="s">
-        <v>396</v>
-      </c>
-      <c r="H149" s="2" t="s">
-        <v>370</v>
-      </c>
-      <c r="I149" s="2" t="s">
+      <c r="K149" s="2" t="s">
         <v>465</v>
       </c>
-      <c r="K149" s="2" t="s">
-        <v>466</v>
-      </c>
       <c r="L149" s="2" t="s">
         <v>370</v>
       </c>
@@ -7858,33 +7858,33 @@
         <v>369</v>
       </c>
       <c r="N149" s="2" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="Q149" s="2" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="150" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A150" s="2" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="B150" s="2" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="E150" s="2" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="H150" s="2" t="s">
         <v>369</v>
       </c>
       <c r="I150" s="2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="J150" s="2" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="K150" s="2" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="L150" s="2" t="s">
         <v>369</v>
@@ -7893,30 +7893,30 @@
         <v>370</v>
       </c>
       <c r="N150" s="2" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="151" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A151" s="2" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="B151" s="2" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="E151" s="2" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="H151" s="2" t="s">
         <v>369</v>
       </c>
       <c r="I151" s="2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="J151" s="2" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="K151" s="2" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="L151" s="2" t="s">
         <v>369</v>
@@ -7925,30 +7925,30 @@
         <v>370</v>
       </c>
       <c r="N151" s="2" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="152" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A152" s="2" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B152" s="2" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="E152" s="2" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="H152" s="2" t="s">
         <v>369</v>
       </c>
       <c r="I152" s="2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="J152" s="2" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="K152" s="2" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="L152" s="2" t="s">
         <v>369</v>
@@ -7957,30 +7957,30 @@
         <v>370</v>
       </c>
       <c r="N152" s="2" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="153" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A153" s="2" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="B153" s="2" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="E153" s="2" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="H153" s="2" t="s">
         <v>369</v>
       </c>
       <c r="I153" s="2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="J153" s="2" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="K153" s="2" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="L153" s="2" t="s">
         <v>369</v>
@@ -7989,27 +7989,27 @@
         <v>370</v>
       </c>
       <c r="N153" s="2" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="154" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A154" s="2" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="B154" s="2" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="E154" s="2" t="s">
+        <v>420</v>
+      </c>
+      <c r="H154" s="2" t="s">
+        <v>369</v>
+      </c>
+      <c r="I154" s="2" t="s">
         <v>421</v>
       </c>
-      <c r="H154" s="2" t="s">
-        <v>369</v>
-      </c>
-      <c r="I154" s="2" t="s">
-        <v>422</v>
-      </c>
       <c r="K154" s="2" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="L154" s="2" t="s">
         <v>369</v>
@@ -8018,24 +8018,24 @@
         <v>370</v>
       </c>
       <c r="N154" s="2" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="155" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A155" s="2" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="B155" s="2" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="E155" s="2" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="H155" s="2" t="s">
         <v>369</v>
       </c>
       <c r="K155" s="2" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="L155" s="2" t="s">
         <v>369</v>
@@ -8044,7 +8044,7 @@
         <v>370</v>
       </c>
       <c r="N155" s="2" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
   </sheetData>

</xml_diff>